<commit_message>
feat: daily templates report
</commit_message>
<xml_diff>
--- a/public/templates/list_template.xlsx
+++ b/public/templates/list_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\proyecto_quisvar\quisvar_proyect_ft\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j1m-1\OneDrive\Documentos\jim\Quisvar\quisvar_proyect_ft\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B8140E-9393-4588-90FE-15FFB25B0C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E941AE3A-D818-4996-B53E-7E60C9B4B668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2A99DD02-9F49-46A8-8BDA-982B4B360E0E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{2A99DD02-9F49-46A8-8BDA-982B4B360E0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -168,7 +168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,25 +201,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor rgb="FFF8C5C5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF87E4BD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
+        <fgColor rgb="FFFFE17F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor rgb="FFF19191"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD2595B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF83A8F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -519,9 +531,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -534,9 +543,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -546,20 +552,8 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -570,27 +564,10 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -600,7 +577,6 @@
     <xf numFmtId="164" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -608,6 +584,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -618,7 +630,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFFFCCCC"/>
+      <color rgb="FF83A8F0"/>
+      <color rgb="FFD2595B"/>
+      <color rgb="FFF19191"/>
+      <color rgb="FFF8C5C5"/>
+      <color rgb="FFFFE17F"/>
+      <color rgb="FF87E4BD"/>
+      <color rgb="FFFFD140"/>
+      <color rgb="FF57D9A3"/>
+      <color rgb="FF2264E5"/>
+      <color rgb="FFC00000"/>
     </mruColors>
   </colors>
   <extLst>
@@ -932,7 +953,7 @@
   <dimension ref="B2:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -954,13 +975,13 @@
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="38"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="40"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
@@ -978,13 +999,13 @@
       <c r="F4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="34"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="36"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="25"/>
     </row>
     <row r="5" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4"/>
@@ -992,25 +1013,25 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="31" t="s">
         <v>14</v>
       </c>
       <c r="I5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="30" t="s">
+      <c r="J5" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="K5" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="32" t="s">
+      <c r="L5" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="33" t="s">
+      <c r="M5" s="21" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1036,107 +1057,107 @@
       <c r="B8" s="9">
         <v>1</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>0</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <v>2</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="15">
         <v>0.5</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="14">
+      <c r="B10" s="13">
         <v>3</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="15">
         <v>10</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="16">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14">
+      <c r="B11" s="13">
         <v>4</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="15">
         <v>20</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="16">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="14">
+      <c r="B12" s="13">
         <v>5</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="15">
         <v>80</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="16">
         <v>160</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="22">
+      <c r="B13" s="17">
         <v>6</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="19">
         <v>0</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P15" s="37"/>
+      <c r="P15" s="22"/>
     </row>
     <row r="16" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>